<commit_message>
Hooked up spiral calc, and repacked the exe for feedback purposes
</commit_message>
<xml_diff>
--- a/Cnc-Calculators-V.2/Database.xlsx
+++ b/Cnc-Calculators-V.2/Database.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>Cutting Meter</t>
   </si>
@@ -29,19 +29,10 @@
     <t>Feed pr Tooth</t>
   </si>
   <si>
-    <t>80</t>
+    <t>0,12</t>
   </si>
   <si>
-    <t>210</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>0.12</t>
-  </si>
-  <si>
-    <t>0,12</t>
+    <t>0,1</t>
   </si>
 </sst>
 </file>
@@ -377,7 +368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:E14"/>
+  <dimension ref="B2:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -400,93 +391,283 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="B3" t="s">
+      <c r="B3" t="n">
+        <v>210</v>
+      </c>
+      <c r="C3" t="n">
+        <v>80</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" t="n">
+        <v>180</v>
+      </c>
+      <c r="C4" t="n">
+        <v>80</v>
+      </c>
+      <c r="D4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" t="n">
+        <v>300</v>
+      </c>
+      <c r="C5" t="n">
+        <v>80</v>
+      </c>
+      <c r="D5" t="n">
         <v>6</v>
       </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B6" t="n">
+        <v>500</v>
+      </c>
+      <c r="C6" t="n">
+        <v>80</v>
+      </c>
+      <c r="D6" t="n">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
+      <c r="B7" t="n">
+        <v>500</v>
+      </c>
+      <c r="C7" t="n">
+        <v>40</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="B8" t="n">
-        <v>210</v>
+        <v>500</v>
+      </c>
+      <c r="C8" t="n">
+        <v>20</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="C9" t="s">
-        <v>4</v>
+      <c r="B9" t="n">
+        <v>40</v>
+      </c>
+      <c r="C9" t="n">
+        <v>20</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" t="n">
-        <v>210</v>
+        <v>60</v>
+      </c>
+      <c r="C10" t="n">
+        <v>20</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5">
+      <c r="B11" t="n">
+        <v>80</v>
+      </c>
       <c r="C11" t="n">
-        <v>80</v>
+        <v>20</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5">
+      <c r="B12" t="n">
+        <v>100</v>
+      </c>
+      <c r="C12" t="n">
+        <v>20</v>
+      </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5">
+      <c r="B13" t="n">
+        <v>120</v>
+      </c>
+      <c r="C13" t="n">
+        <v>20</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="B14" t="s"/>
-      <c r="C14" t="s"/>
-      <c r="D14" t="s"/>
-      <c r="E14" t="n">
-        <v>0.12</v>
+      <c r="B14" t="n">
+        <v>140</v>
+      </c>
+      <c r="C14" t="n">
+        <v>20</v>
+      </c>
+      <c r="D14" t="n">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="B15" t="n">
+        <v>160</v>
+      </c>
+      <c r="C15" t="n">
+        <v>20</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" t="n">
+        <v>180</v>
+      </c>
+      <c r="C16" t="n">
+        <v>20</v>
+      </c>
+      <c r="D16" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="n">
+        <v>200</v>
+      </c>
+      <c r="C17" t="n">
+        <v>20</v>
+      </c>
+      <c r="D17" t="n">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="n">
+        <v>200</v>
+      </c>
+      <c r="C18" t="n">
+        <v>100</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="n">
+        <v>200</v>
+      </c>
+      <c r="C19" t="n">
+        <v>10</v>
+      </c>
+      <c r="D19" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" t="n">
+        <v>10</v>
+      </c>
+      <c r="D20" t="n">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" t="n">
+        <v>10</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" t="n">
+        <v>70</v>
+      </c>
+      <c r="C22" t="n">
+        <v>10</v>
+      </c>
+      <c r="D22" t="n">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Figured out textinput clearing
</commit_message>
<xml_diff>
--- a/Cnc-Calculators-V.2/Database.xlsx
+++ b/Cnc-Calculators-V.2/Database.xlsx
@@ -368,7 +368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:E24"/>
+  <dimension ref="B2:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -698,6 +698,76 @@
         <v>0.12</v>
       </c>
     </row>
+    <row r="25" spans="1:5">
+      <c r="B25" t="n">
+        <v>200</v>
+      </c>
+      <c r="C25" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" t="n">
+        <v>4</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" t="n">
+        <v>150</v>
+      </c>
+      <c r="C26" t="n">
+        <v>5</v>
+      </c>
+      <c r="D26" t="n">
+        <v>4</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" t="n">
+        <v>120</v>
+      </c>
+      <c r="C27" t="n">
+        <v>5</v>
+      </c>
+      <c r="D27" t="n">
+        <v>4</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" t="n">
+        <v>250</v>
+      </c>
+      <c r="C28" t="n">
+        <v>10</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" t="n">
+        <v>250</v>
+      </c>
+      <c r="C29" t="n">
+        <v>10</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Put my modified textinput class in a sep file and added it to the rest
</commit_message>
<xml_diff>
--- a/Cnc-Calculators-V.2/Database.xlsx
+++ b/Cnc-Calculators-V.2/Database.xlsx
@@ -368,7 +368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:E29"/>
+  <dimension ref="B2:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -768,6 +768,202 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="30" spans="1:5">
+      <c r="B30" t="n">
+        <v>120</v>
+      </c>
+      <c r="C30" t="n">
+        <v>40</v>
+      </c>
+      <c r="D30" t="n">
+        <v>4</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" t="n">
+        <v>90</v>
+      </c>
+      <c r="C31" t="n">
+        <v>8</v>
+      </c>
+      <c r="D31" t="n">
+        <v>4</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" t="n">
+        <v>60</v>
+      </c>
+      <c r="C32" t="n">
+        <v>8</v>
+      </c>
+      <c r="D32" t="n">
+        <v>4</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="B33" t="n">
+        <v>40</v>
+      </c>
+      <c r="C33" t="n">
+        <v>8</v>
+      </c>
+      <c r="D33" t="n">
+        <v>4</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="B34" t="n">
+        <v>40</v>
+      </c>
+      <c r="C34" t="n">
+        <v>10</v>
+      </c>
+      <c r="D34" t="n">
+        <v>4</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="B35" t="n">
+        <v>40</v>
+      </c>
+      <c r="C35" t="n">
+        <v>10</v>
+      </c>
+      <c r="D35" t="n">
+        <v>4</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="B36" t="n">
+        <v>30</v>
+      </c>
+      <c r="C36" t="n">
+        <v>10</v>
+      </c>
+      <c r="D36" t="n">
+        <v>4</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="B37" t="n">
+        <v>60</v>
+      </c>
+      <c r="C37" t="n">
+        <v>10</v>
+      </c>
+      <c r="D37" t="n">
+        <v>4</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="B38" t="n">
+        <v>60</v>
+      </c>
+      <c r="C38" t="n">
+        <v>12</v>
+      </c>
+      <c r="D38" t="n">
+        <v>4</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="B39" t="n">
+        <v>210</v>
+      </c>
+      <c r="C39" t="n">
+        <v>80</v>
+      </c>
+      <c r="D39" t="n">
+        <v>6</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="B40" t="n">
+        <v>300</v>
+      </c>
+      <c r="C40" t="n">
+        <v>80</v>
+      </c>
+      <c r="D40" t="n">
+        <v>6</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="B41" t="n">
+        <v>300</v>
+      </c>
+      <c r="C41" t="n">
+        <v>60</v>
+      </c>
+      <c r="D41" t="n">
+        <v>6</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="B42" t="n">
+        <v>300</v>
+      </c>
+      <c r="C42" t="n">
+        <v>60</v>
+      </c>
+      <c r="D42" t="n">
+        <v>4</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="B43" t="n">
+        <v>300</v>
+      </c>
+      <c r="C43" t="n">
+        <v>60</v>
+      </c>
+      <c r="D43" t="n">
+        <v>4</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
added saving of usage data to material removal rate calc and cleaned up some code
</commit_message>
<xml_diff>
--- a/Cnc-Calculators-V.2/Database.xlsx
+++ b/Cnc-Calculators-V.2/Database.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="630" yWindow="510" windowWidth="27495" windowHeight="12720"/>
   </bookViews>
   <sheets>
-    <sheet name="Cutting Speed" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Cutting Speed" sheetId="1" r:id="rId1"/>
+    <sheet name="Material Removal Rate" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Cutting Meter</t>
   </si>
@@ -27,25 +27,39 @@
   </si>
   <si>
     <t>Feed pr Tooth</t>
+  </si>
+  <si>
+    <t>Depth of cut</t>
+  </si>
+  <si>
+    <t>Width of cut</t>
+  </si>
+  <si>
+    <t>Feedrate</t>
+  </si>
+  <si>
+    <t>Material Removal Rate</t>
+  </si>
+  <si>
+    <t>cm³/min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -61,15 +75,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -357,20 +377,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="B2:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -384,91 +404,70 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="B3" t="n">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3">
         <v>210</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>80</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>6</v>
       </c>
-      <c r="E3" t="n">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" t="n">
-        <v>200</v>
-      </c>
-      <c r="C4" t="n">
-        <v>80</v>
-      </c>
-      <c r="D4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5" t="n">
-        <v>190</v>
-      </c>
-      <c r="C5" t="n">
-        <v>80</v>
-      </c>
-      <c r="D5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" t="n">
-        <v>180</v>
-      </c>
-      <c r="C6" t="n">
-        <v>80</v>
-      </c>
-      <c r="D6" t="n">
-        <v>6</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" t="n">
-        <v>50</v>
-      </c>
-      <c r="C7" t="n">
-        <v>80</v>
-      </c>
-      <c r="D7" t="n">
-        <v>6</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>80</v>
-      </c>
-      <c r="D8" t="n">
-        <v>6</v>
-      </c>
-      <c r="E8" t="n">
+      <c r="E3">
         <v>0.12</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>60</v>
+      </c>
+      <c r="D3">
+        <v>602</v>
+      </c>
+      <c r="E3">
+        <v>72.239999999999995</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added datasaving to the spiral module
</commit_message>
<xml_diff>
--- a/Cnc-Calculators-V.2/Database.xlsx
+++ b/Cnc-Calculators-V.2/Database.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Iver\Dokumenter\GitHub\Redesigned_Cnc-Calculators\Cnc-Calculators-V.2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="630" yWindow="510" windowWidth="27495" windowHeight="12720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cutting Speed" sheetId="1" r:id="rId1"/>
     <sheet name="Material Removal Rate" sheetId="2" r:id="rId2"/>
+    <sheet name="Helix Angle" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Cutting Meter</t>
   </si>
@@ -42,12 +48,24 @@
   </si>
   <si>
     <t>cm³/min</t>
+  </si>
+  <si>
+    <t>Hole Diameter</t>
+  </si>
+  <si>
+    <t>Step/Pitch</t>
+  </si>
+  <si>
+    <t>Angle of Decent</t>
+  </si>
+  <si>
+    <t>°</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,6 +106,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -377,12 +398,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -424,12 +445,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
@@ -470,4 +491,56 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B2:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <v>3.04</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
datasaving now added to all modules in the calc, also done some more housekeeping
</commit_message>
<xml_diff>
--- a/Cnc-Calculators-V.2/Database.xlsx
+++ b/Cnc-Calculators-V.2/Database.xlsx
@@ -9,19 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cutting Speed" sheetId="1" r:id="rId1"/>
     <sheet name="Material Removal Rate" sheetId="2" r:id="rId2"/>
     <sheet name="Helix Angle" sheetId="3" r:id="rId3"/>
+    <sheet name="Ramp Angle" sheetId="4" r:id="rId4"/>
+    <sheet name="Surface Roughness" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Cutting Meter</t>
   </si>
@@ -60,6 +62,18 @@
   </si>
   <si>
     <t>°</t>
+  </si>
+  <si>
+    <t>Toolpath Length</t>
+  </si>
+  <si>
+    <t>Feed per Turn</t>
+  </si>
+  <si>
+    <t>Nose Radius</t>
+  </si>
+  <si>
+    <t>Ra</t>
   </si>
 </sst>
 </file>
@@ -399,16 +413,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E3"/>
+  <dimension ref="B2:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
@@ -436,6 +450,20 @@
         <v>6</v>
       </c>
       <c r="E3">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4">
+        <v>80</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
         <v>0.12</v>
       </c>
     </row>
@@ -446,7 +474,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:F3"/>
+  <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -454,7 +482,7 @@
   <cols>
     <col min="2" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
@@ -473,18 +501,35 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>60</v>
       </c>
       <c r="D3">
-        <v>602</v>
+        <v>1000</v>
       </c>
       <c r="E3">
-        <v>72.239999999999995</v>
+        <v>300</v>
       </c>
       <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>600</v>
+      </c>
+      <c r="F4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -495,11 +540,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:F3"/>
+  <dimension ref="B2:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -525,19 +568,243 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="E3">
-        <v>3.04</v>
+        <v>3.65</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="E4">
+        <v>1.82</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>0.06</v>
+      </c>
+      <c r="E5">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B2:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1.72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>150</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>200</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0.86</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="B2:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>10.42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0.3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0.2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0.2</v>
+      </c>
+      <c r="C7">
+        <v>0.2</v>
+      </c>
+      <c r="D7">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0.05</v>
+      </c>
+      <c r="C8">
+        <v>0.2</v>
+      </c>
+      <c r="D8">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0.08</v>
+      </c>
+      <c r="C9">
+        <v>0.2</v>
+      </c>
+      <c r="D9">
+        <v>1.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
we are now dealing with non number inputs, they should never make their way to the excel file
</commit_message>
<xml_diff>
--- a/Cnc-Calculators-V.2/Database.xlsx
+++ b/Cnc-Calculators-V.2/Database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="4"/>
+    <workbookView activeTab="4" windowHeight="12720" windowWidth="27495" xWindow="630" yWindow="510"/>
   </bookViews>
   <sheets>
     <sheet name="Cutting Speed" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Surface Roughness" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>Cutting Meter</t>
   </si>
@@ -35,6 +35,18 @@
     <t>jalla</t>
   </si>
   <si>
+    <t>Hei</t>
+  </si>
+  <si>
+    <t>Ærling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the </t>
+  </si>
+  <si>
+    <t>Lærling</t>
+  </si>
+  <si>
     <t>Depth of cut</t>
   </si>
   <si>
@@ -48,6 +60,12 @@
   </si>
   <si>
     <t>cm³/min</t>
+  </si>
+  <si>
+    <t>ehi</t>
+  </si>
+  <si>
+    <t>Please input values</t>
   </si>
   <si>
     <t>Hole Diameter</t>
@@ -407,13 +425,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:E5"/>
+  <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="2" min="2" width="13.28515625"/>
     <col bestFit="1" customWidth="1" max="3" min="3" width="13.140625"/>
@@ -475,6 +493,76 @@
       </c>
       <c r="E5" t="n">
         <v>0.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>80</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -488,13 +576,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:F4"/>
+  <dimension ref="B2:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="3" min="2" width="11.85546875"/>
     <col bestFit="1" customWidth="1" max="4" min="4" width="9"/>
@@ -503,16 +591,16 @@
   <sheetData>
     <row r="2" spans="1:6">
       <c r="B2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -529,7 +617,7 @@
         <v>300</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -546,7 +634,361 @@
         <v>600</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>60</v>
+      </c>
+      <c r="D5" t="n">
+        <v>602</v>
+      </c>
+      <c r="E5" t="n">
+        <v>36.12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>60</v>
+      </c>
+      <c r="D6" t="n">
+        <v>602</v>
+      </c>
+      <c r="E6" t="n">
+        <v>72.23999999999999</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>60</v>
+      </c>
+      <c r="D7" t="n">
+        <v>602</v>
+      </c>
+      <c r="E7" t="n">
+        <v>36.12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>60</v>
+      </c>
+      <c r="D8" t="n">
+        <v>602</v>
+      </c>
+      <c r="E8" t="n">
+        <v>72.23999999999999</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>60</v>
+      </c>
+      <c r="D9" t="n">
+        <v>602</v>
+      </c>
+      <c r="E9" t="n">
+        <v>36.12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>60</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1208</v>
+      </c>
+      <c r="E10" t="n">
+        <v>72.48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>60</v>
+      </c>
+      <c r="D11" t="n">
+        <v>602</v>
+      </c>
+      <c r="E11" t="n">
+        <v>36.12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>60</v>
+      </c>
+      <c r="D12" t="n">
+        <v>301</v>
+      </c>
+      <c r="E12" t="n">
+        <v>18.06</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>60</v>
+      </c>
+      <c r="D13" t="n">
+        <v>301</v>
+      </c>
+      <c r="E13" t="n">
+        <v>36.12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>60</v>
+      </c>
+      <c r="D14" t="n">
+        <v>301</v>
+      </c>
+      <c r="E14" t="n">
+        <v>18.06</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>60</v>
+      </c>
+      <c r="D15" t="n">
+        <v>602</v>
+      </c>
+      <c r="E15" t="n">
+        <v>36.12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="n">
+        <v>60</v>
+      </c>
+      <c r="D16" t="n">
+        <v>602</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>60</v>
+      </c>
+      <c r="D17" t="n">
+        <v>602</v>
+      </c>
+      <c r="E17" t="n">
+        <v>36.12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>60</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>60</v>
+      </c>
+      <c r="D24" t="n">
+        <v>602</v>
+      </c>
+      <c r="E24" t="n">
+        <v>36.12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>60</v>
+      </c>
+      <c r="D25" t="n">
+        <v>602</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -560,13 +1002,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:F5"/>
+  <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="2" min="2" width="13.140625"/>
     <col bestFit="1" customWidth="1" max="3" min="3" width="13.85546875"/>
@@ -579,13 +1021,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -602,7 +1044,7 @@
         <v>3.65</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -619,7 +1061,7 @@
         <v>1.82</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -636,7 +1078,109 @@
         <v>1.09</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>6</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>6</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -650,13 +1194,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="2" min="2" width="15.28515625"/>
     <col bestFit="1" customWidth="1" max="3" min="3" width="10.28515625"/>
@@ -665,13 +1209,13 @@
   <sheetData>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -685,7 +1229,7 @@
         <v>0.57</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -699,7 +1243,7 @@
         <v>1.72</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -713,7 +1257,7 @@
         <v>1.15</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -727,7 +1271,63 @@
         <v>0.86</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -741,13 +1341,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="2" min="2" width="13.28515625"/>
     <col bestFit="1" customWidth="1" max="3" min="3" width="11.85546875"/>
@@ -755,13 +1355,13 @@
   <sheetData>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -839,6 +1439,39 @@
       </c>
       <c r="D9" t="n">
         <v>1.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PEPified the code, trying to follow established conventions more
</commit_message>
<xml_diff>
--- a/Cnc-Calculators-V.2/Database.xlsx
+++ b/Cnc-Calculators-V.2/Database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="4" windowHeight="12720" windowWidth="27495" xWindow="630" yWindow="510"/>
+    <workbookView activeTab="0" windowHeight="12720" windowWidth="27495" xWindow="630" yWindow="510"/>
   </bookViews>
   <sheets>
     <sheet name="Cutting Speed" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Cutting Meter</t>
   </si>
@@ -32,21 +32,6 @@
     <t>Feed pr Tooth</t>
   </si>
   <si>
-    <t>jalla</t>
-  </si>
-  <si>
-    <t>Hei</t>
-  </si>
-  <si>
-    <t>Ærling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the </t>
-  </si>
-  <si>
-    <t>Lærling</t>
-  </si>
-  <si>
     <t>Depth of cut</t>
   </si>
   <si>
@@ -60,12 +45,6 @@
   </si>
   <si>
     <t>cm³/min</t>
-  </si>
-  <si>
-    <t>ehi</t>
-  </si>
-  <si>
-    <t>Please input values</t>
   </si>
   <si>
     <t>Hole Diameter</t>
@@ -427,8 +406,8 @@
   </sheetPr>
   <dimension ref="B2:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -482,8 +461,8 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="B5" t="s">
-        <v>4</v>
+      <c r="B5" t="n">
+        <v>0</v>
       </c>
       <c r="C5" t="n">
         <v>80</v>
@@ -496,17 +475,17 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>80</v>
+      </c>
+      <c r="D6" t="n">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
+      <c r="E6" t="n">
+        <v>0.12</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -514,13 +493,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -553,16 +532,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="B10" t="n">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>
@@ -576,10 +555,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:F25"/>
+  <dimension ref="B2:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -591,16 +570,16 @@
   <sheetData>
     <row r="2" spans="1:6">
       <c r="B2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -617,7 +596,7 @@
         <v>300</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -634,7 +613,7 @@
         <v>600</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -651,7 +630,7 @@
         <v>36.12</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -668,7 +647,7 @@
         <v>72.23999999999999</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -685,7 +664,7 @@
         <v>36.12</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -702,7 +681,7 @@
         <v>72.23999999999999</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -719,7 +698,7 @@
         <v>36.12</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -736,7 +715,7 @@
         <v>72.48</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -753,7 +732,7 @@
         <v>36.12</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -770,7 +749,7 @@
         <v>18.06</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -787,7 +766,7 @@
         <v>36.12</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -804,7 +783,7 @@
         <v>18.06</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -821,12 +800,12 @@
         <v>36.12</v>
       </c>
       <c r="F15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>14</v>
+      <c r="B16" t="n">
+        <v>0</v>
       </c>
       <c r="C16" t="n">
         <v>60</v>
@@ -834,11 +813,11 @@
       <c r="D16" t="n">
         <v>602</v>
       </c>
-      <c r="E16" t="s">
-        <v>15</v>
+      <c r="E16" t="n">
+        <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -855,7 +834,7 @@
         <v>36.12</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -868,11 +847,11 @@
       <c r="D18" t="n">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
-        <v>15</v>
+      <c r="E18" t="n">
+        <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -886,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -903,7 +882,7 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -920,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -937,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -954,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -971,7 +950,7 @@
         <v>36.12</v>
       </c>
       <c r="F24" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -988,7 +967,24 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>60</v>
+      </c>
+      <c r="D26" t="n">
+        <v>602</v>
+      </c>
+      <c r="E26" t="n">
+        <v>36.12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1005,7 +1001,7 @@
   <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -1021,13 +1017,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1044,7 +1040,7 @@
         <v>3.65</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1061,7 +1057,7 @@
         <v>1.82</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1078,7 +1074,7 @@
         <v>1.09</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1091,11 +1087,11 @@
       <c r="D6" t="n">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
-        <v>15</v>
+      <c r="E6" t="n">
+        <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1112,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1129,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1146,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1163,7 +1159,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1180,7 +1176,7 @@
         <v>1.09</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1197,7 +1193,7 @@
   <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -1209,13 +1205,13 @@
   <sheetData>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1229,7 +1225,7 @@
         <v>0.57</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1243,7 +1239,7 @@
         <v>1.72</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1257,7 +1253,7 @@
         <v>1.15</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1271,7 +1267,7 @@
         <v>0.86</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1281,11 +1277,11 @@
       <c r="C7" t="n">
         <v>0</v>
       </c>
-      <c r="D7" t="s">
-        <v>15</v>
+      <c r="D7" t="n">
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1299,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1313,7 +1309,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1327,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1343,7 +1339,7 @@
   </sheetPr>
   <dimension ref="B2:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1355,13 +1351,13 @@
   <sheetData>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
fixed a small mishapp
</commit_message>
<xml_diff>
--- a/Cnc-Calculators-V.2/Database.xlsx
+++ b/Cnc-Calculators-V.2/Database.xlsx
@@ -404,7 +404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:E10"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -544,6 +544,20 @@
         <v>0.12</v>
       </c>
     </row>
+    <row r="11" spans="1:5">
+      <c r="B11" t="n">
+        <v>210</v>
+      </c>
+      <c r="C11" t="n">
+        <v>80</v>
+      </c>
+      <c r="D11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -555,7 +569,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:F26"/>
+  <dimension ref="B2:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
@@ -987,6 +1001,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="27" spans="1:6">
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>60</v>
+      </c>
+      <c r="D27" t="n">
+        <v>602</v>
+      </c>
+      <c r="E27" t="n">
+        <v>36.12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -998,7 +1029,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:F11"/>
+  <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -1179,6 +1210,23 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12" spans="1:6">
+      <c r="B12" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>6</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1190,7 +1238,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:E10"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -1326,6 +1374,34 @@
         <v>12</v>
       </c>
     </row>
+    <row r="11" spans="1:5">
+      <c r="B11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12" t="n">
+        <v>250</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1337,7 +1413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:D12"/>
+  <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -1470,6 +1546,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="13" spans="1:4">
+      <c r="B13" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2.08</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
made it run on ubuntu
</commit_message>
<xml_diff>
--- a/Cnc-Calculators-V.2/Database.xlsx
+++ b/Cnc-Calculators-V.2/Database.xlsx
@@ -404,7 +404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:E12"/>
+  <dimension ref="B2:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -569,6 +569,20 @@
         <v>6</v>
       </c>
       <c r="E12" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" t="n">
+        <v>210</v>
+      </c>
+      <c r="C13" t="n">
+        <v>80</v>
+      </c>
+      <c r="D13" t="n">
+        <v>6</v>
+      </c>
+      <c r="E13" t="n">
         <v>0.12</v>
       </c>
     </row>

</xml_diff>